<commit_message>
Revert "Merge branch 'Visualisation' of https://github.com/HebemusPapam/PupilCore_Poly into Visualisation"
This reverts commit 5b910ef9f1e32dfc59889fcb981493c735339d29, reversing
changes made to c02d7be712853006e7dbadded3aa8b52b0761b78.
</commit_message>
<xml_diff>
--- a/m n° 001 fixation.xlsx
+++ b/m n° 001 fixation.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,19 +492,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>51.36769866943359</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>100.6277084350586</v>
+        <v>101.071533203125</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3158594965934753</v>
+        <v>0.004170999862253666</v>
       </c>
     </row>
     <row r="3">
@@ -512,19 +512,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-124</v>
+        <v>88</v>
       </c>
       <c r="C3" t="n">
-        <v>115</v>
+        <v>-85</v>
       </c>
       <c r="D3" t="n">
-        <v>50.15015029907227</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>100.9836273193359</v>
+        <v>101.2715530395508</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2254675030708313</v>
+        <v>0.00804550014436245</v>
       </c>
     </row>
     <row r="4">
@@ -532,19 +532,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-127</v>
+        <v>-122</v>
       </c>
       <c r="C4" t="n">
-        <v>-85</v>
+        <v>-74</v>
       </c>
       <c r="D4" t="n">
-        <v>60.27573013305664</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>101.2476119995117</v>
+        <v>101.3976211547852</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9880375266075134</v>
+        <v>0.003957000095397234</v>
       </c>
     </row>
     <row r="5">
@@ -552,19 +552,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-7</v>
+        <v>-118</v>
       </c>
       <c r="C5" t="n">
-        <v>-53</v>
+        <v>-81</v>
       </c>
       <c r="D5" t="n">
-        <v>52.09153747558594</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>102.2756271362305</v>
+        <v>101.4355545043945</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5092869997024536</v>
+        <v>0.004015000071376562</v>
       </c>
     </row>
     <row r="6">
@@ -572,19 +572,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-2</v>
+        <v>124</v>
       </c>
       <c r="C6" t="n">
-        <v>-44</v>
+        <v>-97</v>
       </c>
       <c r="D6" t="n">
-        <v>54.59700393676758</v>
+        <v>150</v>
       </c>
       <c r="E6" t="n">
-        <v>103.0315399169922</v>
+        <v>101.5475769042969</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5700899958610535</v>
+        <v>0.004004000220447779</v>
       </c>
     </row>
     <row r="7">
@@ -592,19 +592,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>127</v>
+        <v>-110</v>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>-78</v>
       </c>
       <c r="D7" t="n">
-        <v>55.92251205444336</v>
+        <v>150</v>
       </c>
       <c r="E7" t="n">
-        <v>103.6436080932617</v>
+        <v>101.6356048583984</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6661540269851685</v>
+        <v>0.003978000022470951</v>
       </c>
     </row>
     <row r="8">
@@ -612,19 +612,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-33</v>
+        <v>-11</v>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>-64</v>
       </c>
       <c r="D8" t="n">
-        <v>52.09153747558594</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>104.3515319824219</v>
+        <v>102.53564453125</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3720965087413788</v>
+        <v>0.003951500169932842</v>
       </c>
     </row>
     <row r="9">
@@ -632,19 +632,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>-123</v>
+        <v>-61</v>
       </c>
       <c r="D9" t="n">
-        <v>51.26511383056641</v>
+        <v>150</v>
       </c>
       <c r="E9" t="n">
-        <v>104.7675094604492</v>
+        <v>102.897590637207</v>
       </c>
       <c r="F9" t="n">
-        <v>0.304064005613327</v>
+        <v>0.003950499929487705</v>
       </c>
     </row>
     <row r="10">
@@ -652,19 +652,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-104</v>
+        <v>-7</v>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>-39</v>
       </c>
       <c r="D10" t="n">
-        <v>51.98751068115234</v>
+        <v>150</v>
       </c>
       <c r="E10" t="n">
-        <v>105.3156051635742</v>
+        <v>103.2675247192383</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3641740083694458</v>
+        <v>0.003983499947935343</v>
       </c>
     </row>
     <row r="11">
@@ -672,19 +672,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-126</v>
+        <v>-17</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>-50</v>
       </c>
       <c r="D11" t="n">
-        <v>50.55275726318359</v>
+        <v>150</v>
       </c>
       <c r="E11" t="n">
-        <v>105.7175521850586</v>
+        <v>103.3236465454102</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2588120102882385</v>
+        <v>0.003966500051319599</v>
       </c>
     </row>
     <row r="12">
@@ -692,19 +692,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>-58</v>
+        <v>-40</v>
       </c>
       <c r="D12" t="n">
-        <v>57.28020095825195</v>
+        <v>150</v>
       </c>
       <c r="E12" t="n">
-        <v>106.017578125</v>
+        <v>103.4796142578125</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7703844904899597</v>
+        <v>0.003964500036090612</v>
       </c>
     </row>
     <row r="13">
@@ -712,19 +712,219 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-112</v>
+        <v>99</v>
       </c>
       <c r="C13" t="n">
-        <v>-76</v>
+        <v>24</v>
       </c>
       <c r="D13" t="n">
-        <v>50.75527191162109</v>
+        <v>150</v>
       </c>
       <c r="E13" t="n">
-        <v>107.2316589355469</v>
+        <v>103.8636474609375</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2600280046463013</v>
+        <v>0.003941500093787909</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-69</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>104.2556228637695</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.004013000056147575</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>17</v>
+      </c>
+      <c r="D15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" t="n">
+        <v>104.531608581543</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.003988500218838453</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>119</v>
+      </c>
+      <c r="C16" t="n">
+        <v>125</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>104.8235626220703</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.004050500225275755</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-128</v>
+      </c>
+      <c r="C17" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" t="n">
+        <v>105.5175094604492</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.006065499968826771</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-118</v>
+      </c>
+      <c r="C18" t="n">
+        <v>19</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>105.887580871582</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.004149000160396099</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-47</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>106.2396697998047</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.004043499939143658</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>14</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-50</v>
+      </c>
+      <c r="D20" t="n">
+        <v>150</v>
+      </c>
+      <c r="E20" t="n">
+        <v>106.4475860595703</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.004038000013679266</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>11</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-58</v>
+      </c>
+      <c r="D21" t="n">
+        <v>150</v>
+      </c>
+      <c r="E21" t="n">
+        <v>106.4714965820312</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.004100500140339136</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>120</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>106.939582824707</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003977499902248383</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>60</v>
+      </c>
+      <c r="C23" t="n">
+        <v>99</v>
+      </c>
+      <c r="D23" t="n">
+        <v>150</v>
+      </c>
+      <c r="E23" t="n">
+        <v>107.1596145629883</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.003966500051319599</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -778,19 +978,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>-126</v>
       </c>
       <c r="D2" t="n">
-        <v>51.16273880004883</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>64.51167297363281</v>
+        <v>64.96161651611328</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2998639941215515</v>
+        <v>0.003996000159531832</v>
       </c>
     </row>
     <row r="3">
@@ -798,19 +998,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" t="n">
-        <v>-100</v>
+        <v>-88</v>
       </c>
       <c r="D3" t="n">
-        <v>57.85558700561523</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>64.85163879394531</v>
+        <v>65.13957977294922</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8110139966011047</v>
+        <v>0.004009000025689602</v>
       </c>
     </row>
     <row r="4">
@@ -818,19 +1018,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-2</v>
+        <v>83</v>
       </c>
       <c r="C4" t="n">
-        <v>-33</v>
+        <v>-94</v>
       </c>
       <c r="D4" t="n">
-        <v>53.24966430664062</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>65.70362091064453</v>
+        <v>65.33563995361328</v>
       </c>
       <c r="F4" t="n">
-        <v>0.462042510509491</v>
+        <v>0.003943500109016895</v>
       </c>
     </row>
     <row r="5">
@@ -838,19 +1038,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="C5" t="n">
-        <v>90</v>
+        <v>-99</v>
       </c>
       <c r="D5" t="n">
-        <v>51.72835159301758</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>66.40760803222656</v>
+        <v>65.35759735107422</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3400270044803619</v>
+        <v>0.004020499996840954</v>
       </c>
     </row>
     <row r="6">
@@ -858,19 +1058,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="C6" t="n">
-        <v>71</v>
+        <v>-108</v>
       </c>
       <c r="D6" t="n">
-        <v>56.54074478149414</v>
+        <v>150</v>
       </c>
       <c r="E6" t="n">
-        <v>66.78765869140625</v>
+        <v>65.51959228515625</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7279419898986816</v>
+        <v>0.004007999785244465</v>
       </c>
     </row>
     <row r="7">
@@ -878,19 +1078,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C7" t="n">
-        <v>70</v>
+        <v>-91</v>
       </c>
       <c r="D7" t="n">
-        <v>51.78007888793945</v>
+        <v>150</v>
       </c>
       <c r="E7" t="n">
-        <v>67.55755615234375</v>
+        <v>65.57573699951172</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3500919938087463</v>
+        <v>0.004067500121891499</v>
       </c>
     </row>
     <row r="8">
@@ -898,19 +1098,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="C8" t="n">
-        <v>-85</v>
+        <v>-96</v>
       </c>
       <c r="D8" t="n">
-        <v>53.62353515625</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>67.95151519775391</v>
+        <v>65.60759735107422</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4960735142230988</v>
+        <v>0.004039499908685684</v>
       </c>
     </row>
     <row r="9">
@@ -918,19 +1118,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-127</v>
+        <v>-12</v>
       </c>
       <c r="C9" t="n">
-        <v>-88</v>
+        <v>-47</v>
       </c>
       <c r="D9" t="n">
-        <v>53.35621643066406</v>
+        <v>150</v>
       </c>
       <c r="E9" t="n">
-        <v>68.49163818359375</v>
+        <v>65.78366088867188</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4722585082054138</v>
+        <v>0.004056000150740147</v>
       </c>
     </row>
     <row r="10">
@@ -938,19 +1138,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="D10" t="n">
-        <v>67.75315856933594</v>
+        <v>150</v>
       </c>
       <c r="E10" t="n">
-        <v>69.007568359375</v>
+        <v>66.28766632080078</v>
       </c>
       <c r="F10" t="n">
-        <v>1.474084973335266</v>
+        <v>0.0039984998293221</v>
       </c>
     </row>
     <row r="11">
@@ -958,19 +1158,439 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
+        <v>108</v>
+      </c>
+      <c r="C11" t="n">
+        <v>78</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="n">
+        <v>66.35159301757812</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.006039999891072512</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>112</v>
+      </c>
+      <c r="C12" t="n">
+        <v>79</v>
+      </c>
+      <c r="D12" t="n">
+        <v>150</v>
+      </c>
+      <c r="E12" t="n">
+        <v>66.40353393554688</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.004073500167578459</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>80</v>
+      </c>
+      <c r="D13" t="n">
+        <v>150</v>
+      </c>
+      <c r="E13" t="n">
+        <v>66.88767242431641</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.003994999919086695</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>79</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>66.89566802978516</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.00395999988541007</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>84</v>
+      </c>
+      <c r="D15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" t="n">
+        <v>66.93565368652344</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.003899999894201756</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>110</v>
+      </c>
+      <c r="C16" t="n">
+        <v>84</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>67.56157684326172</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.004017000086605549</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>36</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-93</v>
+      </c>
+      <c r="D17" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" t="n">
+        <v>68.10760498046875</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.00395999988541007</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-127</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-91</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>68.80753326416016</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.004036500118672848</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>47</v>
+      </c>
+      <c r="C19" t="n">
+        <v>29</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>69.13957214355469</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.004077500198036432</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>43</v>
+      </c>
+      <c r="C20" t="n">
+        <v>46</v>
+      </c>
+      <c r="D20" t="n">
+        <v>150</v>
+      </c>
+      <c r="E20" t="n">
+        <v>69.48765563964844</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.003998999949544668</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>47</v>
+      </c>
+      <c r="C21" t="n">
+        <v>34</v>
+      </c>
+      <c r="D21" t="n">
+        <v>150</v>
+      </c>
+      <c r="E21" t="n">
+        <v>69.67767333984375</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.006062000058591366</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>46</v>
+      </c>
+      <c r="C22" t="n">
+        <v>21</v>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>69.92764282226562</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003949000034481287</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>41</v>
+      </c>
+      <c r="C23" t="n">
+        <v>25</v>
+      </c>
+      <c r="D23" t="n">
+        <v>150</v>
+      </c>
+      <c r="E23" t="n">
+        <v>70.25157928466797</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.004038000013679266</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>16</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-114</v>
+      </c>
+      <c r="D24" t="n">
+        <v>150</v>
+      </c>
+      <c r="E24" t="n">
+        <v>70.70766448974609</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.004019000101834536</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>30</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-114</v>
+      </c>
+      <c r="D25" t="n">
+        <v>150</v>
+      </c>
+      <c r="E25" t="n">
+        <v>70.76961517333984</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.004095999989658594</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>37</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-99</v>
+      </c>
+      <c r="D26" t="n">
+        <v>150</v>
+      </c>
+      <c r="E26" t="n">
+        <v>70.88767242431641</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.003980999812483788</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-95</v>
+      </c>
+      <c r="D27" t="n">
+        <v>150</v>
+      </c>
+      <c r="E27" t="n">
+        <v>71.15152740478516</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.004050500225275755</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-80</v>
+      </c>
+      <c r="D28" t="n">
+        <v>150</v>
+      </c>
+      <c r="E28" t="n">
+        <v>71.20359802246094</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.003966500051319599</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="C11" t="n">
-        <v>-97</v>
-      </c>
-      <c r="D11" t="n">
-        <v>59.97525405883789</v>
-      </c>
-      <c r="E11" t="n">
-        <v>70.52758026123047</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.9560545086860657</v>
+      <c r="B29" t="n">
+        <v>30</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-82</v>
+      </c>
+      <c r="D29" t="n">
+        <v>150</v>
+      </c>
+      <c r="E29" t="n">
+        <v>71.21560668945312</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.003973999992012978</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>32</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-106</v>
+      </c>
+      <c r="D30" t="n">
+        <v>150</v>
+      </c>
+      <c r="E30" t="n">
+        <v>71.29169464111328</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.003958499990403652</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>23</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-98</v>
+      </c>
+      <c r="D31" t="n">
+        <v>150</v>
+      </c>
+      <c r="E31" t="n">
+        <v>71.39161682128906</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.003992999903857708</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>28</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-96</v>
+      </c>
+      <c r="D32" t="n">
+        <v>150</v>
+      </c>
+      <c r="E32" t="n">
+        <v>71.45555877685547</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.00405499991029501</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +1604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1024,19 +1644,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="C2" t="n">
-        <v>-20</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>53.24966430664062</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>76.51158905029297</v>
+        <v>76.69963073730469</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4800625145435333</v>
+        <v>0.004009999800473452</v>
       </c>
     </row>
     <row r="3">
@@ -1044,19 +1664,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-108</v>
+        <v>-99</v>
       </c>
       <c r="C3" t="n">
-        <v>-104</v>
+        <v>-87</v>
       </c>
       <c r="D3" t="n">
-        <v>80.94599151611328</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>77.03556060791016</v>
+        <v>77.09162902832031</v>
       </c>
       <c r="F3" t="n">
-        <v>2.231969594955444</v>
+        <v>0.004050999879837036</v>
       </c>
     </row>
     <row r="4">
@@ -1064,19 +1684,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>63</v>
+        <v>-104</v>
       </c>
       <c r="C4" t="n">
-        <v>-118</v>
+        <v>-77</v>
       </c>
       <c r="D4" t="n">
-        <v>68.57068634033203</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>79.33167266845703</v>
+        <v>77.18965911865234</v>
       </c>
       <c r="F4" t="n">
-        <v>1.545969009399414</v>
+        <v>0.005929999984800816</v>
       </c>
     </row>
     <row r="5">
@@ -1084,19 +1704,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-88</v>
+        <v>-107</v>
       </c>
       <c r="C5" t="n">
-        <v>-96</v>
+        <v>-100</v>
       </c>
       <c r="D5" t="n">
-        <v>67.95662689208984</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>80.91960144042969</v>
+        <v>77.50369262695312</v>
       </c>
       <c r="F5" t="n">
-        <v>1.497077465057373</v>
+        <v>0.004007000010460615</v>
       </c>
     </row>
     <row r="6">
@@ -1104,19 +1724,379 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="C6" t="n">
-        <v>-95</v>
+        <v>-122</v>
       </c>
       <c r="D6" t="n">
-        <v>60.69892883300781</v>
+        <v>150</v>
       </c>
       <c r="E6" t="n">
-        <v>82.45558929443359</v>
+        <v>77.96758270263672</v>
       </c>
       <c r="F6" t="n">
-        <v>1.012009978294373</v>
+        <v>0.006052500102669001</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-120</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-108</v>
+      </c>
+      <c r="D7" t="n">
+        <v>150</v>
+      </c>
+      <c r="E7" t="n">
+        <v>78.00788116455078</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.004015000071376562</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-102</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-119</v>
+      </c>
+      <c r="D8" t="n">
+        <v>150</v>
+      </c>
+      <c r="E8" t="n">
+        <v>78.41558074951172</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.003981499932706356</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-106</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-113</v>
+      </c>
+      <c r="D9" t="n">
+        <v>150</v>
+      </c>
+      <c r="E9" t="n">
+        <v>78.46365356445312</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.003948499914258718</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-107</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-118</v>
+      </c>
+      <c r="D10" t="n">
+        <v>150</v>
+      </c>
+      <c r="E10" t="n">
+        <v>78.49568939208984</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.00400950014591217</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-84</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-105</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="n">
+        <v>78.56358337402344</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.004031499847769737</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-121</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-119</v>
+      </c>
+      <c r="D12" t="n">
+        <v>150</v>
+      </c>
+      <c r="E12" t="n">
+        <v>78.78560638427734</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.009963000193238258</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-102</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-119</v>
+      </c>
+      <c r="D13" t="n">
+        <v>150</v>
+      </c>
+      <c r="E13" t="n">
+        <v>79.01563262939453</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.003926500212401152</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>64</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-116</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>79.64386749267578</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.00397850014269352</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>35</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-128</v>
+      </c>
+      <c r="D15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" t="n">
+        <v>79.81553649902344</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.004008499905467033</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>43</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-128</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>79.83957672119141</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.004064499866217375</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>63</v>
+      </c>
+      <c r="C17" t="n">
+        <v>120</v>
+      </c>
+      <c r="D17" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" t="n">
+        <v>79.95565795898438</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.003970500081777573</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>67</v>
+      </c>
+      <c r="C18" t="n">
+        <v>105</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>80.12762451171875</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.004025499802082777</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>51</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-119</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>80.24760437011719</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.00395999988541007</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-104</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-97</v>
+      </c>
+      <c r="D20" t="n">
+        <v>150</v>
+      </c>
+      <c r="E20" t="n">
+        <v>81.00364685058594</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.008030000142753124</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-109</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-103</v>
+      </c>
+      <c r="D21" t="n">
+        <v>150</v>
+      </c>
+      <c r="E21" t="n">
+        <v>81.04360198974609</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.004023000132292509</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-81</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-97</v>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>81.46366882324219</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003898999886587262</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-73</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-90</v>
+      </c>
+      <c r="D23" t="n">
+        <v>150</v>
+      </c>
+      <c r="E23" t="n">
+        <v>81.56754302978516</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.006071500014513731</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>-99</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-111</v>
+      </c>
+      <c r="D24" t="n">
+        <v>150</v>
+      </c>
+      <c r="E24" t="n">
+        <v>81.94773101806641</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.003804000094532967</v>
       </c>
     </row>
   </sheetData>
@@ -1130,7 +2110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1170,19 +2150,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C2" t="n">
-        <v>-14</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>57.68236923217773</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>52.42767333984375</v>
+        <v>52.47159194946289</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7999929785728455</v>
+        <v>0.004042500164359808</v>
       </c>
     </row>
     <row r="3">
@@ -1190,19 +2170,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-86</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>-60</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>54.27056503295898</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>53.4715461730957</v>
+        <v>52.65755844116211</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5408340096473694</v>
+        <v>0.00400350010022521</v>
       </c>
     </row>
     <row r="4">
@@ -1210,19 +2190,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-39</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>56.82401657104492</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>54.05363082885742</v>
+        <v>52.69963073730469</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7619234919548035</v>
+        <v>0.003982500173151493</v>
       </c>
     </row>
     <row r="5">
@@ -1230,19 +2210,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-43</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>-87</v>
+        <v>-35</v>
       </c>
       <c r="D5" t="n">
-        <v>61.67742919921875</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>54.85762405395508</v>
+        <v>52.89172744750977</v>
       </c>
       <c r="F5" t="n">
-        <v>1.08187997341156</v>
+        <v>0.004025000147521496</v>
       </c>
     </row>
     <row r="6">
@@ -1250,19 +2230,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-44</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>-99</v>
+        <v>-31</v>
       </c>
       <c r="D6" t="n">
-        <v>57.33748245239258</v>
+        <v>150</v>
       </c>
       <c r="E6" t="n">
-        <v>55.97964096069336</v>
+        <v>53.11166381835938</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7779120206832886</v>
+        <v>0.0039470000192523</v>
       </c>
     </row>
     <row r="7">
@@ -1270,19 +2250,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>56</v>
+        <v>-7</v>
       </c>
       <c r="C7" t="n">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D7" t="n">
-        <v>53.67715835571289</v>
+        <v>150</v>
       </c>
       <c r="E7" t="n">
-        <v>56.79959869384766</v>
+        <v>54.13158798217773</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5360394716262817</v>
+        <v>0.003989499993622303</v>
       </c>
     </row>
     <row r="8">
@@ -1290,19 +2270,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>-64</v>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>-107</v>
       </c>
       <c r="D8" t="n">
-        <v>53.7308349609375</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>57.57965469360352</v>
+        <v>54.89971160888672</v>
       </c>
       <c r="F8" t="n">
-        <v>0.503958523273468</v>
+        <v>0.004019000101834536</v>
       </c>
     </row>
     <row r="9">
@@ -1310,19 +2290,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-108</v>
+        <v>-53</v>
       </c>
       <c r="C9" t="n">
-        <v>73</v>
+        <v>-97</v>
       </c>
       <c r="D9" t="n">
-        <v>52.09153747558594</v>
+        <v>150</v>
       </c>
       <c r="E9" t="n">
-        <v>58.1276969909668</v>
+        <v>55.11163330078125</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3719800114631653</v>
+        <v>0.003969999961555004</v>
       </c>
     </row>
     <row r="10">
@@ -1330,19 +2310,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>32</v>
+        <v>-55</v>
       </c>
       <c r="C10" t="n">
-        <v>29</v>
+        <v>-101</v>
       </c>
       <c r="D10" t="n">
-        <v>55.42171859741211</v>
+        <v>150</v>
       </c>
       <c r="E10" t="n">
-        <v>58.54354476928711</v>
+        <v>55.1995849609375</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6369199752807617</v>
+        <v>0.00395999988541007</v>
       </c>
     </row>
     <row r="11">
@@ -1350,19 +2330,279 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
+        <v>-50</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-54</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="n">
+        <v>55.4356575012207</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.003978999797254801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-29</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-87</v>
+      </c>
+      <c r="D12" t="n">
+        <v>150</v>
+      </c>
+      <c r="E12" t="n">
+        <v>55.71564483642578</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.003971999976783991</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-39</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-93</v>
+      </c>
+      <c r="D13" t="n">
+        <v>150</v>
+      </c>
+      <c r="E13" t="n">
+        <v>55.77556991577148</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.004002999980002642</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-68</v>
+      </c>
+      <c r="C14" t="n">
+        <v>127</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>56.0716438293457</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.00399750005453825</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-35</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-76</v>
+      </c>
+      <c r="D15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" t="n">
+        <v>56.33948516845703</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.004048500210046768</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>41</v>
+      </c>
+      <c r="C16" t="n">
+        <v>85</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>56.9316291809082</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.003949000034481287</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="C11" t="n">
-        <v>-56</v>
-      </c>
-      <c r="D11" t="n">
-        <v>50.50225448608398</v>
-      </c>
-      <c r="E11" t="n">
-        <v>59.22359466552734</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.2420080006122589</v>
+      <c r="B17" t="n">
+        <v>68</v>
+      </c>
+      <c r="C17" t="n">
+        <v>97</v>
+      </c>
+      <c r="D17" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" t="n">
+        <v>57.19168090820312</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.003978999797254801</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>103</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>57.80764770507812</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.003992499783635139</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>96</v>
+      </c>
+      <c r="C19" t="n">
+        <v>22</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>57.84365844726562</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.006018000189214945</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>81</v>
+      </c>
+      <c r="C20" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" t="n">
+        <v>150</v>
+      </c>
+      <c r="E20" t="n">
+        <v>58.03558731079102</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.004037499893456697</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-100</v>
+      </c>
+      <c r="C21" t="n">
+        <v>78</v>
+      </c>
+      <c r="D21" t="n">
+        <v>150</v>
+      </c>
+      <c r="E21" t="n">
+        <v>58.28763961791992</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.003984000068157911</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>46</v>
+      </c>
+      <c r="C22" t="n">
+        <v>35</v>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>58.52366256713867</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003992999903857708</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>46</v>
+      </c>
+      <c r="C23" t="n">
+        <v>37</v>
+      </c>
+      <c r="D23" t="n">
+        <v>150</v>
+      </c>
+      <c r="E23" t="n">
+        <v>58.57560348510742</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.003993500024080276</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>32</v>
+      </c>
+      <c r="C24" t="n">
+        <v>16</v>
+      </c>
+      <c r="D24" t="n">
+        <v>150</v>
+      </c>
+      <c r="E24" t="n">
+        <v>58.88767242431641</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.004033999983221292</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +2616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1416,19 +2656,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="n">
         <v>26</v>
       </c>
-      <c r="C2" t="n">
-        <v>28</v>
-      </c>
       <c r="D2" t="n">
-        <v>51.72835159301758</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>88.61160278320312</v>
+        <v>88.62348937988281</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3399355113506317</v>
+        <v>0.004096500109881163</v>
       </c>
     </row>
     <row r="3">
@@ -1436,19 +2676,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-58</v>
+        <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>-41</v>
+        <v>27</v>
       </c>
       <c r="D3" t="n">
-        <v>51.06056594848633</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>88.99355316162109</v>
+        <v>88.63553619384766</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3269815146923065</v>
+        <v>0.004038999788463116</v>
       </c>
     </row>
     <row r="4">
@@ -1456,19 +2696,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>-100</v>
+        <v>35</v>
       </c>
       <c r="D4" t="n">
-        <v>55.14543914794922</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>89.36356353759766</v>
+        <v>88.81954956054688</v>
       </c>
       <c r="F4" t="n">
-        <v>0.614031970500946</v>
+        <v>0.0040480000898242</v>
       </c>
     </row>
     <row r="5">
@@ -1476,19 +2716,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-73</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>-90</v>
+        <v>31</v>
       </c>
       <c r="D5" t="n">
-        <v>54.98033142089844</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>90.01957702636719</v>
+        <v>88.83564758300781</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5960224866867065</v>
+        <v>0.004000999964773655</v>
       </c>
     </row>
     <row r="6">
@@ -1496,19 +2736,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>114</v>
+        <v>-72</v>
       </c>
       <c r="C6" t="n">
-        <v>-69</v>
+        <v>-36</v>
       </c>
       <c r="D6" t="n">
-        <v>51.88369369506836</v>
+        <v>150</v>
       </c>
       <c r="E6" t="n">
-        <v>90.65567016601562</v>
+        <v>89.15560150146484</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3638460040092468</v>
+        <v>0.003996999934315681</v>
       </c>
     </row>
     <row r="7">
@@ -1516,19 +2756,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-32</v>
+        <v>124</v>
       </c>
       <c r="C7" t="n">
-        <v>-82</v>
+        <v>-122</v>
       </c>
       <c r="D7" t="n">
-        <v>52.98421478271484</v>
+        <v>150</v>
       </c>
       <c r="E7" t="n">
-        <v>91.06359100341797</v>
+        <v>89.49968719482422</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4440990090370178</v>
+        <v>0.004024500027298927</v>
       </c>
     </row>
     <row r="8">
@@ -1536,19 +2776,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-122</v>
+        <v>-79</v>
       </c>
       <c r="C8" t="n">
-        <v>-118</v>
+        <v>-106</v>
       </c>
       <c r="D8" t="n">
-        <v>56.20268630981445</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>91.55156707763672</v>
+        <v>90.0716552734375</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7159860134124756</v>
+        <v>0.004043499939143658</v>
       </c>
     </row>
     <row r="9">
@@ -1556,19 +2796,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>-87</v>
       </c>
       <c r="C9" t="n">
-        <v>101</v>
+        <v>-103</v>
       </c>
       <c r="D9" t="n">
-        <v>50.30075073242188</v>
+        <v>150</v>
       </c>
       <c r="E9" t="n">
-        <v>92.30767059326172</v>
+        <v>90.41961669921875</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2279594987630844</v>
+        <v>0.008019000291824341</v>
       </c>
     </row>
     <row r="10">
@@ -1576,19 +2816,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>119</v>
+        <v>-88</v>
       </c>
       <c r="C10" t="n">
-        <v>114</v>
+        <v>-99</v>
       </c>
       <c r="D10" t="n">
-        <v>59.91534042358398</v>
+        <v>150</v>
       </c>
       <c r="E10" t="n">
-        <v>92.97968292236328</v>
+        <v>90.43959808349609</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9729815125465393</v>
+        <v>0.004118000157177448</v>
       </c>
     </row>
     <row r="11">
@@ -1596,19 +2836,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-17</v>
+        <v>-78</v>
       </c>
       <c r="C11" t="n">
-        <v>126</v>
+        <v>-91</v>
       </c>
       <c r="D11" t="n">
-        <v>59.85548400878906</v>
+        <v>150</v>
       </c>
       <c r="E11" t="n">
-        <v>93.99353790283203</v>
+        <v>90.48567962646484</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9499905109405518</v>
+        <v>0.003975499887019396</v>
       </c>
     </row>
     <row r="12">
@@ -1616,19 +2856,519 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
+        <v>104</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-55</v>
+      </c>
+      <c r="D12" t="n">
+        <v>150</v>
+      </c>
+      <c r="E12" t="n">
+        <v>90.68960571289062</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.004025499802082777</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>116</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-68</v>
+      </c>
+      <c r="D13" t="n">
+        <v>150</v>
+      </c>
+      <c r="E13" t="n">
+        <v>90.98358917236328</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.006049999967217445</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-120</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-120</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>91.54768371582031</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.00388449989259243</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-116</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-123</v>
+      </c>
+      <c r="D15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" t="n">
+        <v>91.56358337402344</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.004002999980002642</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>96</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>92.27564239501953</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.003963499795645475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-87</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-109</v>
+      </c>
+      <c r="D17" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" t="n">
+        <v>92.63559722900391</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.003965499810874462</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-109</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-124</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>92.73953247070312</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.004048500210046768</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-89</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-94</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>92.88961791992188</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.004031499847769737</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-117</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D20" t="n">
+        <v>150</v>
+      </c>
+      <c r="E20" t="n">
+        <v>93.07154083251953</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.004095999989658594</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
         <v>119</v>
       </c>
-      <c r="C12" t="n">
-        <v>101</v>
-      </c>
-      <c r="D12" t="n">
-        <v>54.21635055541992</v>
-      </c>
-      <c r="E12" t="n">
-        <v>94.98200225830078</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.5416374802589417</v>
+      <c r="C21" t="n">
+        <v>110</v>
+      </c>
+      <c r="D21" t="n">
+        <v>150</v>
+      </c>
+      <c r="E21" t="n">
+        <v>93.36365509033203</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.003955000080168247</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>108</v>
+      </c>
+      <c r="C22" t="n">
+        <v>102</v>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>93.57970428466797</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003922999836504459</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>108</v>
+      </c>
+      <c r="C23" t="n">
+        <v>95</v>
+      </c>
+      <c r="D23" t="n">
+        <v>150</v>
+      </c>
+      <c r="E23" t="n">
+        <v>93.77959442138672</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.004027499817311764</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>105</v>
+      </c>
+      <c r="C24" t="n">
+        <v>95</v>
+      </c>
+      <c r="D24" t="n">
+        <v>150</v>
+      </c>
+      <c r="E24" t="n">
+        <v>93.84364318847656</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.003955999854952097</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>99</v>
+      </c>
+      <c r="C25" t="n">
+        <v>98</v>
+      </c>
+      <c r="D25" t="n">
+        <v>150</v>
+      </c>
+      <c r="E25" t="n">
+        <v>93.85556793212891</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.003996000159531832</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>7</v>
+      </c>
+      <c r="C26" t="n">
+        <v>124</v>
+      </c>
+      <c r="D26" t="n">
+        <v>150</v>
+      </c>
+      <c r="E26" t="n">
+        <v>94.01554870605469</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.004062000196427107</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-10</v>
+      </c>
+      <c r="C27" t="n">
+        <v>123</v>
+      </c>
+      <c r="D27" t="n">
+        <v>150</v>
+      </c>
+      <c r="E27" t="n">
+        <v>94.06364440917969</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.007902000099420547</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-11</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-115</v>
+      </c>
+      <c r="D28" t="n">
+        <v>150</v>
+      </c>
+      <c r="E28" t="n">
+        <v>94.12362670898438</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.004018499981611967</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C29" t="n">
+        <v>120</v>
+      </c>
+      <c r="D29" t="n">
+        <v>150</v>
+      </c>
+      <c r="E29" t="n">
+        <v>94.42762756347656</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.003945000004023314</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-39</v>
+      </c>
+      <c r="C30" t="n">
+        <v>125</v>
+      </c>
+      <c r="D30" t="n">
+        <v>150</v>
+      </c>
+      <c r="E30" t="n">
+        <v>94.85565948486328</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.004009000025689602</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-111</v>
+      </c>
+      <c r="C31" t="n">
+        <v>124</v>
+      </c>
+      <c r="D31" t="n">
+        <v>150</v>
+      </c>
+      <c r="E31" t="n">
+        <v>94.9478759765625</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.004091000184416771</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-100</v>
+      </c>
+      <c r="C32" t="n">
+        <v>117</v>
+      </c>
+      <c r="D32" t="n">
+        <v>150</v>
+      </c>
+      <c r="E32" t="n">
+        <v>94.95571899414062</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.004980499856173992</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-112</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-128</v>
+      </c>
+      <c r="D33" t="n">
+        <v>150</v>
+      </c>
+      <c r="E33" t="n">
+        <v>94.96460723876953</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.004357500001788139</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-108</v>
+      </c>
+      <c r="C34" t="n">
+        <v>125</v>
+      </c>
+      <c r="D34" t="n">
+        <v>150</v>
+      </c>
+      <c r="E34" t="n">
+        <v>94.97309112548828</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.004943499807268381</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-105</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-125</v>
+      </c>
+      <c r="D35" t="n">
+        <v>150</v>
+      </c>
+      <c r="E35" t="n">
+        <v>94.99217224121094</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.005111000034958124</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-101</v>
+      </c>
+      <c r="C36" t="n">
+        <v>123</v>
+      </c>
+      <c r="D36" t="n">
+        <v>150</v>
+      </c>
+      <c r="E36" t="n">
+        <v>95.00131225585938</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.003922999836504459</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>109</v>
+      </c>
+      <c r="C37" t="n">
+        <v>103</v>
+      </c>
+      <c r="D37" t="n">
+        <v>150</v>
+      </c>
+      <c r="E37" t="n">
+        <v>95.0596923828125</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.003921499941498041</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +3382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1682,19 +3422,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C2" t="n">
-        <v>-3</v>
+        <v>-12</v>
       </c>
       <c r="D2" t="n">
-        <v>51.06056594848633</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>112.7435684204102</v>
+        <v>112.8396072387695</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3024545013904572</v>
+        <v>0.004011000040918589</v>
       </c>
     </row>
     <row r="3">
@@ -1702,19 +3442,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-116</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>-80</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>65.42396545410156</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>113.087646484375</v>
+        <v>112.9036178588867</v>
       </c>
       <c r="F3" t="n">
-        <v>1.319961547851562</v>
+        <v>0.003990999888628721</v>
       </c>
     </row>
     <row r="4">
@@ -1722,19 +3462,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="C4" t="n">
-        <v>127</v>
+        <v>-80</v>
       </c>
       <c r="D4" t="n">
-        <v>71.29638671875</v>
+        <v>150</v>
       </c>
       <c r="E4" t="n">
-        <v>114.4515686035156</v>
+        <v>113.4136505126953</v>
       </c>
       <c r="F4" t="n">
-        <v>1.752097010612488</v>
+        <v>0.003974500112235546</v>
       </c>
     </row>
     <row r="5">
@@ -1742,19 +3482,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-67</v>
+        <v>-91</v>
       </c>
       <c r="C5" t="n">
-        <v>126</v>
+        <v>-98</v>
       </c>
       <c r="D5" t="n">
-        <v>58.96479415893555</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>116.4476699829102</v>
+        <v>113.5835647583008</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8975589871406555</v>
+        <v>0.004038000013679266</v>
       </c>
     </row>
     <row r="6">
@@ -1762,19 +3502,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>114</v>
+        <v>-108</v>
       </c>
       <c r="C6" t="n">
-        <v>-20</v>
+        <v>-69</v>
       </c>
       <c r="D6" t="n">
-        <v>51.93557739257812</v>
+        <v>150</v>
       </c>
       <c r="E6" t="n">
-        <v>117.3876495361328</v>
+        <v>113.7715606689453</v>
       </c>
       <c r="F6" t="n">
-        <v>0.36387699842453</v>
+        <v>0.004015500191599131</v>
       </c>
     </row>
     <row r="7">
@@ -1782,19 +3522,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-38</v>
+        <v>-110</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>-82</v>
       </c>
       <c r="D7" t="n">
-        <v>55.86664581298828</v>
+        <v>150</v>
       </c>
       <c r="E7" t="n">
-        <v>117.7955932617188</v>
+        <v>114.0396118164062</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6640459895133972</v>
+        <v>0.003990999888628721</v>
       </c>
     </row>
     <row r="8">
@@ -1802,19 +3542,399 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>-112</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-78</v>
+      </c>
+      <c r="D8" t="n">
+        <v>150</v>
+      </c>
+      <c r="E8" t="n">
+        <v>114.0917129516602</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.003950499929487705</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-107</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-77</v>
+      </c>
+      <c r="D9" t="n">
+        <v>150</v>
+      </c>
+      <c r="E9" t="n">
+        <v>114.1035842895508</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.00402349978685379</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-115</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-74</v>
+      </c>
+      <c r="D10" t="n">
+        <v>150</v>
+      </c>
+      <c r="E10" t="n">
+        <v>114.255615234375</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.004182499833405018</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-112</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-74</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="n">
+        <v>114.2916259765625</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.00401049992069602</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>74</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-116</v>
+      </c>
+      <c r="D12" t="n">
+        <v>150</v>
+      </c>
+      <c r="E12" t="n">
+        <v>114.4795989990234</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.003982000052928925</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>55</v>
+      </c>
+      <c r="C13" t="n">
+        <v>124</v>
+      </c>
+      <c r="D13" t="n">
+        <v>150</v>
+      </c>
+      <c r="E13" t="n">
+        <v>114.5395660400391</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.004005500115454197</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
         <v>56</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C14" t="n">
+        <v>122</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>114.5915603637695</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.004028500057756901</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>68</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-116</v>
+      </c>
+      <c r="D15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E15" t="n">
+        <v>114.7256622314453</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.004037499893456697</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>44</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-108</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>114.9876327514648</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.003963499795645475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>77</v>
+      </c>
+      <c r="C17" t="n">
+        <v>126</v>
+      </c>
+      <c r="D17" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" t="n">
+        <v>115.4675674438477</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.003971499856561422</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>47</v>
+      </c>
+      <c r="C18" t="n">
+        <v>116</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>115.5596160888672</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.003956499975174665</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>56</v>
+      </c>
+      <c r="C19" t="n">
+        <v>113</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>115.9595947265625</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.003983499947935343</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
-        <v>57.05165481567383</v>
-      </c>
-      <c r="E8" t="n">
-        <v>118.9037017822266</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.7559124827384949</v>
+      <c r="B20" t="n">
+        <v>49</v>
+      </c>
+      <c r="C20" t="n">
+        <v>121</v>
+      </c>
+      <c r="D20" t="n">
+        <v>150</v>
+      </c>
+      <c r="E20" t="n">
+        <v>116.1395568847656</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.004031499847769737</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-85</v>
+      </c>
+      <c r="C21" t="n">
+        <v>124</v>
+      </c>
+      <c r="D21" t="n">
+        <v>150</v>
+      </c>
+      <c r="E21" t="n">
+        <v>116.7718353271484</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.003930999897420406</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-59</v>
+      </c>
+      <c r="C22" t="n">
+        <v>121</v>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>117.2636260986328</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003936000168323517</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>94</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-20</v>
+      </c>
+      <c r="D23" t="n">
+        <v>150</v>
+      </c>
+      <c r="E23" t="n">
+        <v>117.3796081542969</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.004015500191599131</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>-29</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-16</v>
+      </c>
+      <c r="D24" t="n">
+        <v>150</v>
+      </c>
+      <c r="E24" t="n">
+        <v>117.9555969238281</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.00399750005453825</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-34</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-12</v>
+      </c>
+      <c r="D25" t="n">
+        <v>150</v>
+      </c>
+      <c r="E25" t="n">
+        <v>117.9795761108398</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.004015999846160412</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>114</v>
+      </c>
+      <c r="C26" t="n">
+        <v>62</v>
+      </c>
+      <c r="D26" t="n">
+        <v>150</v>
+      </c>
+      <c r="E26" t="n">
+        <v>118.7036895751953</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.003019500058144331</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>71</v>
+      </c>
+      <c r="C27" t="n">
+        <v>20</v>
+      </c>
+      <c r="D27" t="n">
+        <v>150</v>
+      </c>
+      <c r="E27" t="n">
+        <v>119.6317901611328</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.003854000009596348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>